<commit_message>
Plot create a list and save perfect
</commit_message>
<xml_diff>
--- a/test_ECG_One.xlsx
+++ b/test_ECG_One.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:GR1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -423,7 +423,604 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="n">
-        <v>1</v>
+        <v>0.2879278424498841</v>
+      </c>
+      <c r="B1" t="n">
+        <v>3.032917448393836</v>
+      </c>
+      <c r="C1" t="n">
+        <v>6.938970245718306</v>
+      </c>
+      <c r="D1" t="n">
+        <v>2.493783375877912</v>
+      </c>
+      <c r="E1" t="n">
+        <v>-2.995270403835879</v>
+      </c>
+      <c r="F1" t="n">
+        <v>0.6948393950982852</v>
+      </c>
+      <c r="G1" t="n">
+        <v>0.7394121453760447</v>
+      </c>
+      <c r="H1" t="n">
+        <v>-0.7206583099386735</v>
+      </c>
+      <c r="I1" t="n">
+        <v>0.2952621049829379</v>
+      </c>
+      <c r="J1" t="n">
+        <v>-0.01405880052535969</v>
+      </c>
+      <c r="K1" t="n">
+        <v>-0.04718997084873428</v>
+      </c>
+      <c r="L1" t="n">
+        <v>0.02394257247877265</v>
+      </c>
+      <c r="M1" t="n">
+        <v>-0.01037649250415691</v>
+      </c>
+      <c r="N1" t="n">
+        <v>-0.003362951114676107</v>
+      </c>
+      <c r="O1" t="n">
+        <v>-0.006064602598763074</v>
+      </c>
+      <c r="P1" t="n">
+        <v>-0.007005432771582604</v>
+      </c>
+      <c r="Q1" t="n">
+        <v>-0.007690920394071835</v>
+      </c>
+      <c r="R1" t="n">
+        <v>-0.007853487662263799</v>
+      </c>
+      <c r="S1" t="n">
+        <v>-0.007520062784727445</v>
+      </c>
+      <c r="T1" t="n">
+        <v>-0.006538336452917392</v>
+      </c>
+      <c r="U1" t="n">
+        <v>-0.005042965124975457</v>
+      </c>
+      <c r="V1" t="n">
+        <v>-0.005644444484741967</v>
+      </c>
+      <c r="W1" t="n">
+        <v>0.1193836586237704</v>
+      </c>
+      <c r="X1" t="n">
+        <v>2.142589354558359</v>
+      </c>
+      <c r="Y1" t="n">
+        <v>6.537308950517367</v>
+      </c>
+      <c r="Z1" t="n">
+        <v>4.013883587304656</v>
+      </c>
+      <c r="AA1" t="n">
+        <v>-2.810369122857558</v>
+      </c>
+      <c r="AB1" t="n">
+        <v>-0.1783083145468346</v>
+      </c>
+      <c r="AC1" t="n">
+        <v>1.202822945543864</v>
+      </c>
+      <c r="AD1" t="n">
+        <v>-0.7648134506890276</v>
+      </c>
+      <c r="AE1" t="n">
+        <v>0.1863514912270723</v>
+      </c>
+      <c r="AF1" t="n">
+        <v>0.1050827153474672</v>
+      </c>
+      <c r="AG1" t="n">
+        <v>-0.05115597191426362</v>
+      </c>
+      <c r="AH1" t="n">
+        <v>0.06581558645874597</v>
+      </c>
+      <c r="AI1" t="n">
+        <v>0.02787109061872233</v>
+      </c>
+      <c r="AJ1" t="n">
+        <v>0.03458704495000398</v>
+      </c>
+      <c r="AK1" t="n">
+        <v>0.03325003650916205</v>
+      </c>
+      <c r="AL1" t="n">
+        <v>0.03195498336738942</v>
+      </c>
+      <c r="AM1" t="n">
+        <v>0.0305350760698017</v>
+      </c>
+      <c r="AN1" t="n">
+        <v>0.02901215442620252</v>
+      </c>
+      <c r="AO1" t="n">
+        <v>0.0274566739142957</v>
+      </c>
+      <c r="AP1" t="n">
+        <v>0.02604979282823462</v>
+      </c>
+      <c r="AQ1" t="n">
+        <v>0.02450848151018079</v>
+      </c>
+      <c r="AR1" t="n">
+        <v>0.02290785875039067</v>
+      </c>
+      <c r="AS1" t="n">
+        <v>0.06383970180522841</v>
+      </c>
+      <c r="AT1" t="n">
+        <v>1.475386962855712</v>
+      </c>
+      <c r="AU1" t="n">
+        <v>5.872993496273643</v>
+      </c>
+      <c r="AV1" t="n">
+        <v>5.333397155806427</v>
+      </c>
+      <c r="AW1" t="n">
+        <v>-2.095310167379633</v>
+      </c>
+      <c r="AX1" t="n">
+        <v>-1.136864475573328</v>
+      </c>
+      <c r="AY1" t="n">
+        <v>1.514371498797921</v>
+      </c>
+      <c r="AZ1" t="n">
+        <v>-0.6449400995861141</v>
+      </c>
+      <c r="BA1" t="n">
+        <v>-0.0160447930745535</v>
+      </c>
+      <c r="BB1" t="n">
+        <v>0.2040583317148431</v>
+      </c>
+      <c r="BC1" t="n">
+        <v>-0.09007244294328869</v>
+      </c>
+      <c r="BD1" t="n">
+        <v>0.04832853965322076</v>
+      </c>
+      <c r="BE1" t="n">
+        <v>0.01317275063257317</v>
+      </c>
+      <c r="BF1" t="n">
+        <v>0.0132844872075507</v>
+      </c>
+      <c r="BG1" t="n">
+        <v>0.01345575309082657</v>
+      </c>
+      <c r="BH1" t="n">
+        <v>0.01211923159448598</v>
+      </c>
+      <c r="BI1" t="n">
+        <v>0.01161613040952726</v>
+      </c>
+      <c r="BJ1" t="n">
+        <v>0.01139004027759088</v>
+      </c>
+      <c r="BK1" t="n">
+        <v>0.01157132618470781</v>
+      </c>
+      <c r="BL1" t="n">
+        <v>0.0122542220780253</v>
+      </c>
+      <c r="BM1" t="n">
+        <v>0.01317657183563622</v>
+      </c>
+      <c r="BN1" t="n">
+        <v>0.0156101422390157</v>
+      </c>
+      <c r="BO1" t="n">
+        <v>0.02521554324277021</v>
+      </c>
+      <c r="BP1" t="n">
+        <v>0.9526453569076508</v>
+      </c>
+      <c r="BQ1" t="n">
+        <v>5.018754302587544</v>
+      </c>
+      <c r="BR1" t="n">
+        <v>6.325353833813528</v>
+      </c>
+      <c r="BS1" t="n">
+        <v>-0.8966397435844226</v>
+      </c>
+      <c r="BT1" t="n">
+        <v>-2.007738965737333</v>
+      </c>
+      <c r="BU1" t="n">
+        <v>1.617657392656283</v>
+      </c>
+      <c r="BV1" t="n">
+        <v>-0.3014375577098529</v>
+      </c>
+      <c r="BW1" t="n">
+        <v>-0.2344806920501045</v>
+      </c>
+      <c r="BX1" t="n">
+        <v>0.3167776174047591</v>
+      </c>
+      <c r="BY1" t="n">
+        <v>-0.07681729084640107</v>
+      </c>
+      <c r="BZ1" t="n">
+        <v>0.05248783836127721</v>
+      </c>
+      <c r="CA1" t="n">
+        <v>0.03559061894168424</v>
+      </c>
+      <c r="CB1" t="n">
+        <v>0.02591304722487427</v>
+      </c>
+      <c r="CC1" t="n">
+        <v>0.02802539807802646</v>
+      </c>
+      <c r="CD1" t="n">
+        <v>0.02484477442153892</v>
+      </c>
+      <c r="CE1" t="n">
+        <v>0.02237797673367005</v>
+      </c>
+      <c r="CF1" t="n">
+        <v>0.0193884612670739</v>
+      </c>
+      <c r="CG1" t="n">
+        <v>0.0160844349142653</v>
+      </c>
+      <c r="CH1" t="n">
+        <v>0.01249940108260895</v>
+      </c>
+      <c r="CI1" t="n">
+        <v>0.008692539503934954</v>
+      </c>
+      <c r="CJ1" t="n">
+        <v>0.00610949055217495</v>
+      </c>
+      <c r="CK1" t="n">
+        <v>0.0008619409777932104</v>
+      </c>
+      <c r="CL1" t="n">
+        <v>0.5561196817615569</v>
+      </c>
+      <c r="CM1" t="n">
+        <v>4.062997468131182</v>
+      </c>
+      <c r="CN1" t="n">
+        <v>6.866550896033129</v>
+      </c>
+      <c r="CO1" t="n">
+        <v>0.5707160048941489</v>
+      </c>
+      <c r="CP1" t="n">
+        <v>-2.688986790148954</v>
+      </c>
+      <c r="CQ1" t="n">
+        <v>1.375844116272831</v>
+      </c>
+      <c r="CR1" t="n">
+        <v>0.1281084350731251</v>
+      </c>
+      <c r="CS1" t="n">
+        <v>-0.5082173384948858</v>
+      </c>
+      <c r="CT1" t="n">
+        <v>0.3395070639815334</v>
+      </c>
+      <c r="CU1" t="n">
+        <v>-0.07484990559751233</v>
+      </c>
+      <c r="CV1" t="n">
+        <v>0.00956163754987658</v>
+      </c>
+      <c r="CW1" t="n">
+        <v>0.03423356566892873</v>
+      </c>
+      <c r="CX1" t="n">
+        <v>0.02001031138729089</v>
+      </c>
+      <c r="CY1" t="n">
+        <v>0.03186978974283947</v>
+      </c>
+      <c r="CZ1" t="n">
+        <v>0.03476109224555073</v>
+      </c>
+      <c r="DA1" t="n">
+        <v>0.03813670751986356</v>
+      </c>
+      <c r="DB1" t="n">
+        <v>0.04000128542408804</v>
+      </c>
+      <c r="DC1" t="n">
+        <v>0.04053416581157884</v>
+      </c>
+      <c r="DD1" t="n">
+        <v>0.03986575077276759</v>
+      </c>
+      <c r="DE1" t="n">
+        <v>0.03828337683606883</v>
+      </c>
+      <c r="DF1" t="n">
+        <v>0.0365863320554034</v>
+      </c>
+      <c r="DG1" t="n">
+        <v>0.02969087900995633</v>
+      </c>
+      <c r="DH1" t="n">
+        <v>0.3307435676920188</v>
+      </c>
+      <c r="DI1" t="n">
+        <v>3.161966342729339</v>
+      </c>
+      <c r="DJ1" t="n">
+        <v>6.978948355473086</v>
+      </c>
+      <c r="DK1" t="n">
+        <v>2.217865129695226</v>
+      </c>
+      <c r="DL1" t="n">
+        <v>-2.978732648905749</v>
+      </c>
+      <c r="DM1" t="n">
+        <v>0.8293359326217759</v>
+      </c>
+      <c r="DN1" t="n">
+        <v>0.6581544865175085</v>
+      </c>
+      <c r="DO1" t="n">
+        <v>-0.6878379502443823</v>
+      </c>
+      <c r="DP1" t="n">
+        <v>0.3219318112651099</v>
+      </c>
+      <c r="DQ1" t="n">
+        <v>-0.01034361246111098</v>
+      </c>
+      <c r="DR1" t="n">
+        <v>-0.01940987449060063</v>
+      </c>
+      <c r="DS1" t="n">
+        <v>0.04882568489419184</v>
+      </c>
+      <c r="DT1" t="n">
+        <v>0.02177475009122067</v>
+      </c>
+      <c r="DU1" t="n">
+        <v>0.03451821951901787</v>
+      </c>
+      <c r="DV1" t="n">
+        <v>0.03765331088426607</v>
+      </c>
+      <c r="DW1" t="n">
+        <v>0.04262683286272918</v>
+      </c>
+      <c r="DX1" t="n">
+        <v>0.04767323033671755</v>
+      </c>
+      <c r="DY1" t="n">
+        <v>0.05283484566834083</v>
+      </c>
+      <c r="DZ1" t="n">
+        <v>0.05782130077737613</v>
+      </c>
+      <c r="EA1" t="n">
+        <v>0.06252351830631808</v>
+      </c>
+      <c r="EB1" t="n">
+        <v>0.06662732381297808</v>
+      </c>
+      <c r="EC1" t="n">
+        <v>0.06675581318038414</v>
+      </c>
+      <c r="ED1" t="n">
+        <v>0.211369021990414</v>
+      </c>
+      <c r="EE1" t="n">
+        <v>2.348338186791202</v>
+      </c>
+      <c r="EF1" t="n">
+        <v>6.694412841132394</v>
+      </c>
+      <c r="EG1" t="n">
+        <v>3.82154269114285</v>
+      </c>
+      <c r="EH1" t="n">
+        <v>-2.82674034862071</v>
+      </c>
+      <c r="EI1" t="n">
+        <v>0.02560632153172512</v>
+      </c>
+      <c r="EJ1" t="n">
+        <v>1.163065809265233</v>
+      </c>
+      <c r="EK1" t="n">
+        <v>-0.7457519449646375</v>
+      </c>
+      <c r="EL1" t="n">
+        <v>0.223652961555777</v>
+      </c>
+      <c r="EM1" t="n">
+        <v>0.08686974886531118</v>
+      </c>
+      <c r="EN1" t="n">
+        <v>-0.05377449801541131</v>
+      </c>
+      <c r="EO1" t="n">
+        <v>0.05061803818264074</v>
+      </c>
+      <c r="EP1" t="n">
+        <v>0.009272493083362563</v>
+      </c>
+      <c r="EQ1" t="n">
+        <v>0.01541782799955795</v>
+      </c>
+      <c r="ER1" t="n">
+        <v>0.0157489105472473</v>
+      </c>
+      <c r="ES1" t="n">
+        <v>0.01933817694688515</v>
+      </c>
+      <c r="ET1" t="n">
+        <v>0.02512562839607424</v>
+      </c>
+      <c r="EU1" t="n">
+        <v>0.03257801327591208</v>
+      </c>
+      <c r="EV1" t="n">
+        <v>0.04112881550720682</v>
+      </c>
+      <c r="EW1" t="n">
+        <v>0.05034061713167021</v>
+      </c>
+      <c r="EX1" t="n">
+        <v>0.05931141114150257</v>
+      </c>
+      <c r="EY1" t="n">
+        <v>0.06712857477572612</v>
+      </c>
+      <c r="EZ1" t="n">
+        <v>0.1266566551540786</v>
+      </c>
+      <c r="FA1" t="n">
+        <v>1.641665372352978</v>
+      </c>
+      <c r="FB1" t="n">
+        <v>6.070940695961876</v>
+      </c>
+      <c r="FC1" t="n">
+        <v>5.19394232633665</v>
+      </c>
+      <c r="FD1" t="n">
+        <v>-2.190116598211169</v>
+      </c>
+      <c r="FE1" t="n">
+        <v>-0.9068040418132981</v>
+      </c>
+      <c r="FF1" t="n">
+        <v>1.535246547036871</v>
+      </c>
+      <c r="FG1" t="n">
+        <v>-0.6254761766738116</v>
+      </c>
+      <c r="FH1" t="n">
+        <v>0.07291091417540338</v>
+      </c>
+      <c r="FI1" t="n">
+        <v>0.2315845224758989</v>
+      </c>
+      <c r="FJ1" t="n">
+        <v>-0.0456056376160079</v>
+      </c>
+      <c r="FK1" t="n">
+        <v>0.08602638922231602</v>
+      </c>
+      <c r="FL1" t="n">
+        <v>0.04520452243953552</v>
+      </c>
+      <c r="FM1" t="n">
+        <v>0.04354435253025005</v>
+      </c>
+      <c r="FN1" t="n">
+        <v>0.04132621755980136</v>
+      </c>
+      <c r="FO1" t="n">
+        <v>0.0389108258020147</v>
+      </c>
+      <c r="FP1" t="n">
+        <v>0.0378988495447191</v>
+      </c>
+      <c r="FQ1" t="n">
+        <v>0.0376329863491967</v>
+      </c>
+      <c r="FR1" t="n">
+        <v>0.03801710978197621</v>
+      </c>
+      <c r="FS1" t="n">
+        <v>0.03894818654167803</v>
+      </c>
+      <c r="FT1" t="n">
+        <v>0.03997273071447922</v>
+      </c>
+      <c r="FU1" t="n">
+        <v>0.04220312297866679</v>
+      </c>
+      <c r="FV1" t="n">
+        <v>0.05504986803119841</v>
+      </c>
+      <c r="FW1" t="n">
+        <v>1.05763052184469</v>
+      </c>
+      <c r="FX1" t="n">
+        <v>5.199544025677681</v>
+      </c>
+      <c r="FY1" t="n">
+        <v>6.205543357081423</v>
+      </c>
+      <c r="FZ1" t="n">
+        <v>-1.107276770096579</v>
+      </c>
+      <c r="GA1" t="n">
+        <v>-1.847057985764238</v>
+      </c>
+      <c r="GB1" t="n">
+        <v>1.641030220863206</v>
+      </c>
+      <c r="GC1" t="n">
+        <v>-0.3518980021502474</v>
+      </c>
+      <c r="GD1" t="n">
+        <v>-0.1753806005020255</v>
+      </c>
+      <c r="GE1" t="n">
+        <v>0.3178290131689149</v>
+      </c>
+      <c r="GF1" t="n">
+        <v>-0.06448130468333391</v>
+      </c>
+      <c r="GG1" t="n">
+        <v>0.06717822795715045</v>
+      </c>
+      <c r="GH1" t="n">
+        <v>0.04353006753603979</v>
+      </c>
+      <c r="GI1" t="n">
+        <v>0.03293513282372772</v>
+      </c>
+      <c r="GJ1" t="n">
+        <v>0.03166293214847855</v>
+      </c>
+      <c r="GK1" t="n">
+        <v>0.02580736574857726</v>
+      </c>
+      <c r="GL1" t="n">
+        <v>0.02088867782995732</v>
+      </c>
+      <c r="GM1" t="n">
+        <v>0.01597930428327508</v>
+      </c>
+      <c r="GN1" t="n">
+        <v>0.01146124331564931</v>
+      </c>
+      <c r="GO1" t="n">
+        <v>0.007560044156005212</v>
+      </c>
+      <c r="GP1" t="n">
+        <v>0.004495512400127485</v>
+      </c>
+      <c r="GQ1" t="n">
+        <v>0.002492407963564571</v>
+      </c>
+      <c r="GR1" t="n">
+        <v>0.001774904954790893</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Plot create a list and save correct now
</commit_message>
<xml_diff>
--- a/test_ECG_One.xlsx
+++ b/test_ECG_One.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:GR1"/>
+  <dimension ref="A1:SF1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -423,604 +423,1504 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="n">
-        <v>0.2879278424498841</v>
+        <v>1.115034503403323</v>
       </c>
       <c r="B1" t="n">
-        <v>3.032917448393836</v>
+        <v>0.6784273053693061</v>
       </c>
       <c r="C1" t="n">
-        <v>6.938970245718306</v>
+        <v>0.06698835435431198</v>
       </c>
       <c r="D1" t="n">
-        <v>2.493783375877912</v>
+        <v>-0.113260751681409</v>
       </c>
       <c r="E1" t="n">
-        <v>-2.995270403835879</v>
+        <v>0.004725574766366763</v>
       </c>
       <c r="F1" t="n">
-        <v>0.6948393950982852</v>
+        <v>0.1058830281938421</v>
       </c>
       <c r="G1" t="n">
-        <v>0.7394121453760447</v>
+        <v>0.1318214969248819</v>
       </c>
       <c r="H1" t="n">
-        <v>-0.7206583099386735</v>
+        <v>0.1429239516100592</v>
       </c>
       <c r="I1" t="n">
-        <v>0.2952621049829379</v>
+        <v>0.1582756021334658</v>
       </c>
       <c r="J1" t="n">
-        <v>-0.01405880052535969</v>
+        <v>0.18067519574671</v>
       </c>
       <c r="K1" t="n">
-        <v>-0.04718997084873428</v>
+        <v>0.2121877813890183</v>
       </c>
       <c r="L1" t="n">
-        <v>0.02394257247877265</v>
+        <v>0.2535595324566011</v>
       </c>
       <c r="M1" t="n">
-        <v>-0.01037649250415691</v>
+        <v>0.3043838153912794</v>
       </c>
       <c r="N1" t="n">
-        <v>-0.003362951114676107</v>
+        <v>0.3621320882680187</v>
       </c>
       <c r="O1" t="n">
-        <v>-0.006064602598763074</v>
+        <v>0.4193504778294347</v>
       </c>
       <c r="P1" t="n">
-        <v>-0.007005432771582604</v>
+        <v>0.4690184868076837</v>
       </c>
       <c r="Q1" t="n">
-        <v>-0.007690920394071835</v>
+        <v>0.5050757598448279</v>
       </c>
       <c r="R1" t="n">
-        <v>-0.007853487662263799</v>
+        <v>0.5224159446987438</v>
       </c>
       <c r="S1" t="n">
-        <v>-0.007520062784727445</v>
+        <v>0.5167882796360799</v>
       </c>
       <c r="T1" t="n">
-        <v>-0.006538336452917392</v>
+        <v>0.4871460225128578</v>
       </c>
       <c r="U1" t="n">
-        <v>-0.005042965124975457</v>
+        <v>0.4409462114254677</v>
       </c>
       <c r="V1" t="n">
-        <v>-0.005644444484741967</v>
+        <v>0.3858926591530832</v>
       </c>
       <c r="W1" t="n">
-        <v>0.1193836586237704</v>
+        <v>0.3285543281509972</v>
       </c>
       <c r="X1" t="n">
-        <v>2.142589354558359</v>
+        <v>0.2743653305506213</v>
       </c>
       <c r="Y1" t="n">
-        <v>6.537308950517367</v>
+        <v>0.2276249281594883</v>
       </c>
       <c r="Z1" t="n">
-        <v>4.013883587304656</v>
+        <v>0.1914768906474035</v>
       </c>
       <c r="AA1" t="n">
-        <v>-2.810369122857558</v>
+        <v>0.166514545307839</v>
       </c>
       <c r="AB1" t="n">
-        <v>-0.1783083145468346</v>
+        <v>0.1505350020018418</v>
       </c>
       <c r="AC1" t="n">
-        <v>1.202822945543864</v>
+        <v>0.1413541295199043</v>
       </c>
       <c r="AD1" t="n">
-        <v>-0.7648134506890276</v>
+        <v>0.1370707971690767</v>
       </c>
       <c r="AE1" t="n">
-        <v>0.1863514912270723</v>
+        <v>0.1360680562590231</v>
       </c>
       <c r="AF1" t="n">
-        <v>0.1050827153474672</v>
+        <v>0.1370267187587967</v>
       </c>
       <c r="AG1" t="n">
-        <v>-0.05115597191426362</v>
+        <v>0.1389279721999892</v>
       </c>
       <c r="AH1" t="n">
-        <v>0.06581558645874597</v>
+        <v>0.1412728778393792</v>
       </c>
       <c r="AI1" t="n">
-        <v>0.02787109061872233</v>
+        <v>0.1438167566992685</v>
       </c>
       <c r="AJ1" t="n">
-        <v>0.03458704495000398</v>
+        <v>0.1463752511575563</v>
       </c>
       <c r="AK1" t="n">
-        <v>0.03325003650916205</v>
+        <v>0.1488747620201519</v>
       </c>
       <c r="AL1" t="n">
-        <v>0.03195498336738942</v>
+        <v>0.1513524485209749</v>
       </c>
       <c r="AM1" t="n">
-        <v>0.0305350760698017</v>
+        <v>0.1539562283219549</v>
       </c>
       <c r="AN1" t="n">
-        <v>0.02901215442620252</v>
+        <v>0.156944777513032</v>
       </c>
       <c r="AO1" t="n">
-        <v>0.0274566739142957</v>
+        <v>0.160425604356105</v>
       </c>
       <c r="AP1" t="n">
-        <v>0.02604979282823462</v>
+        <v>0.1669590743533447</v>
       </c>
       <c r="AQ1" t="n">
-        <v>0.02450848151018079</v>
+        <v>0.1806604207657449</v>
       </c>
       <c r="AR1" t="n">
-        <v>0.02290785875039067</v>
+        <v>0.2051415534593584</v>
       </c>
       <c r="AS1" t="n">
-        <v>0.06383970180522841</v>
+        <v>0.2435042956168679</v>
       </c>
       <c r="AT1" t="n">
-        <v>1.475386962855712</v>
+        <v>0.2977961156529727</v>
       </c>
       <c r="AU1" t="n">
-        <v>5.872993496273643</v>
+        <v>0.3569321064811049</v>
       </c>
       <c r="AV1" t="n">
-        <v>5.333397155806427</v>
+        <v>0.4023971390196382</v>
       </c>
       <c r="AW1" t="n">
-        <v>-2.095310167379633</v>
+        <v>0.4204444968053908</v>
       </c>
       <c r="AX1" t="n">
-        <v>-1.136864475573328</v>
+        <v>0.4025409910476075</v>
       </c>
       <c r="AY1" t="n">
-        <v>1.514371498797921</v>
+        <v>0.3550960317586318</v>
       </c>
       <c r="AZ1" t="n">
-        <v>-0.6449400995861141</v>
+        <v>0.2984269523189527</v>
       </c>
       <c r="BA1" t="n">
-        <v>-0.0160447930745535</v>
+        <v>0.2478299602261289</v>
       </c>
       <c r="BB1" t="n">
-        <v>0.2040583317148431</v>
+        <v>0.2122106628142836</v>
       </c>
       <c r="BC1" t="n">
-        <v>-0.09007244294328869</v>
+        <v>0.1947490016553112</v>
       </c>
       <c r="BD1" t="n">
-        <v>0.04832853965322076</v>
+        <v>0.1709536543576142</v>
       </c>
       <c r="BE1" t="n">
-        <v>0.01317275063257317</v>
+        <v>0.1177627491615615</v>
       </c>
       <c r="BF1" t="n">
-        <v>0.0132844872075507</v>
+        <v>0.0346813600876943</v>
       </c>
       <c r="BG1" t="n">
-        <v>0.01345575309082657</v>
+        <v>0.1517108602150747</v>
       </c>
       <c r="BH1" t="n">
-        <v>0.01211923159448598</v>
+        <v>0.6576251883662096</v>
       </c>
       <c r="BI1" t="n">
-        <v>0.01161613040952726</v>
+        <v>1.163687156825391</v>
       </c>
       <c r="BJ1" t="n">
-        <v>0.01139004027759088</v>
+        <v>0.8608061824581248</v>
       </c>
       <c r="BK1" t="n">
-        <v>0.01157132618470781</v>
+        <v>0.212098356413682</v>
       </c>
       <c r="BL1" t="n">
-        <v>0.0122542220780253</v>
+        <v>-0.03265451599887192</v>
       </c>
       <c r="BM1" t="n">
-        <v>0.01317657183563622</v>
+        <v>0.06398789498610914</v>
       </c>
       <c r="BN1" t="n">
-        <v>0.0156101422390157</v>
+        <v>0.1719612192283854</v>
       </c>
       <c r="BO1" t="n">
-        <v>0.02521554324277021</v>
+        <v>0.2060895984130061</v>
       </c>
       <c r="BP1" t="n">
-        <v>0.9526453569076508</v>
+        <v>0.2167588607170743</v>
       </c>
       <c r="BQ1" t="n">
-        <v>5.018754302587544</v>
+        <v>0.2303957397567362</v>
       </c>
       <c r="BR1" t="n">
-        <v>6.325353833813528</v>
+        <v>0.2533035408436464</v>
       </c>
       <c r="BS1" t="n">
-        <v>-0.8966397435844226</v>
+        <v>0.2844217812832938</v>
       </c>
       <c r="BT1" t="n">
-        <v>-2.007738965737333</v>
+        <v>0.3256179248985778</v>
       </c>
       <c r="BU1" t="n">
-        <v>1.617657392656283</v>
+        <v>0.3760627587584564</v>
       </c>
       <c r="BV1" t="n">
-        <v>-0.3014375577098529</v>
+        <v>0.4330620359492701</v>
       </c>
       <c r="BW1" t="n">
-        <v>-0.2344806920501045</v>
+        <v>0.4911263413142236</v>
       </c>
       <c r="BX1" t="n">
-        <v>0.3167776174047591</v>
+        <v>0.5417364848536963</v>
       </c>
       <c r="BY1" t="n">
-        <v>-0.07681729084640107</v>
+        <v>0.5778806641226893</v>
       </c>
       <c r="BZ1" t="n">
-        <v>0.05248783836127721</v>
+        <v>0.5943439871398558</v>
       </c>
       <c r="CA1" t="n">
-        <v>0.03559061894168424</v>
+        <v>0.5875341871978577</v>
       </c>
       <c r="CB1" t="n">
-        <v>0.02591304722487427</v>
+        <v>0.5560486529276406</v>
       </c>
       <c r="CC1" t="n">
-        <v>0.02802539807802646</v>
+        <v>0.5079020786595281</v>
       </c>
       <c r="CD1" t="n">
-        <v>0.02484477442153892</v>
+        <v>0.4516475427046468</v>
       </c>
       <c r="CE1" t="n">
-        <v>0.02237797673367005</v>
+        <v>0.3942433270483908</v>
       </c>
       <c r="CF1" t="n">
-        <v>0.0193884612670739</v>
+        <v>0.3410529173504241</v>
       </c>
       <c r="CG1" t="n">
-        <v>0.0160844349142653</v>
+        <v>0.2958450029446764</v>
       </c>
       <c r="CH1" t="n">
-        <v>0.01249940108260895</v>
+        <v>0.2607934768393453</v>
       </c>
       <c r="CI1" t="n">
-        <v>0.008692539503934954</v>
+        <v>0.236450743995354</v>
       </c>
       <c r="CJ1" t="n">
-        <v>0.00610949055217495</v>
+        <v>0.2211857478606811</v>
       </c>
       <c r="CK1" t="n">
-        <v>0.0008619409777932104</v>
+        <v>0.2125326818609166</v>
       </c>
       <c r="CL1" t="n">
-        <v>0.5561196817615569</v>
+        <v>0.2084130231972749</v>
       </c>
       <c r="CM1" t="n">
-        <v>4.062997468131182</v>
+        <v>0.2071702983834219</v>
       </c>
       <c r="CN1" t="n">
-        <v>6.866550896033129</v>
+        <v>0.2075599054992676</v>
       </c>
       <c r="CO1" t="n">
-        <v>0.5707160048941489</v>
+        <v>0.20874479319081</v>
       </c>
       <c r="CP1" t="n">
-        <v>-2.688986790148954</v>
+        <v>0.2102954663512135</v>
       </c>
       <c r="CQ1" t="n">
-        <v>1.375844116272831</v>
+        <v>0.2120584173763943</v>
       </c>
       <c r="CR1" t="n">
-        <v>0.1281084350731251</v>
+        <v>0.2138095288236445</v>
       </c>
       <c r="CS1" t="n">
-        <v>-0.5082173384948858</v>
+        <v>0.2154375627776812</v>
       </c>
       <c r="CT1" t="n">
-        <v>0.3395070639815334</v>
+        <v>0.2169983982816541</v>
       </c>
       <c r="CU1" t="n">
-        <v>-0.07484990559751233</v>
+        <v>0.2187150313371453</v>
       </c>
       <c r="CV1" t="n">
-        <v>0.00956163754987658</v>
+        <v>0.2209775749041695</v>
       </c>
       <c r="CW1" t="n">
-        <v>0.03423356566892873</v>
+        <v>0.2243828767663771</v>
       </c>
       <c r="CX1" t="n">
-        <v>0.02001031138729089</v>
+        <v>0.2318236200050232</v>
       </c>
       <c r="CY1" t="n">
-        <v>0.03186978974283947</v>
+        <v>0.2474636042758861</v>
       </c>
       <c r="CZ1" t="n">
-        <v>0.03476109224555073</v>
+        <v>0.2753747914539383</v>
       </c>
       <c r="DA1" t="n">
-        <v>0.03813670751986356</v>
+        <v>0.3196738138818581</v>
       </c>
       <c r="DB1" t="n">
-        <v>0.04000128542408804</v>
+        <v>0.3766590261000603</v>
       </c>
       <c r="DC1" t="n">
-        <v>0.04053416581157884</v>
+        <v>0.4300586691747046</v>
       </c>
       <c r="DD1" t="n">
-        <v>0.03986575077276759</v>
+        <v>0.4644555199079115</v>
       </c>
       <c r="DE1" t="n">
-        <v>0.03828337683606883</v>
+        <v>0.4663315001737289</v>
       </c>
       <c r="DF1" t="n">
-        <v>0.0365863320554034</v>
+        <v>0.4302533203244363</v>
       </c>
       <c r="DG1" t="n">
-        <v>0.02969087900995633</v>
+        <v>0.3749979403716763</v>
       </c>
       <c r="DH1" t="n">
-        <v>0.3307435676920188</v>
+        <v>0.3191578075560636</v>
       </c>
       <c r="DI1" t="n">
-        <v>3.161966342729339</v>
+        <v>0.2744971072576258</v>
       </c>
       <c r="DJ1" t="n">
-        <v>6.978948355473086</v>
+        <v>0.2461516137920957</v>
       </c>
       <c r="DK1" t="n">
-        <v>2.217865129695226</v>
+        <v>0.2316823621830965</v>
       </c>
       <c r="DL1" t="n">
-        <v>-2.978732648905749</v>
+        <v>0.19291754180849</v>
       </c>
       <c r="DM1" t="n">
-        <v>0.8293359326217759</v>
+        <v>0.1158097782070444</v>
       </c>
       <c r="DN1" t="n">
-        <v>0.6581544865175085</v>
+        <v>0.08945689805237443</v>
       </c>
       <c r="DO1" t="n">
-        <v>-0.6878379502443823</v>
+        <v>0.4464921915735541</v>
       </c>
       <c r="DP1" t="n">
-        <v>0.3219318112651099</v>
+        <v>1.052614343539449</v>
       </c>
       <c r="DQ1" t="n">
-        <v>-0.01034361246111098</v>
+        <v>1.115773699798524</v>
       </c>
       <c r="DR1" t="n">
-        <v>-0.01940987449060063</v>
+        <v>0.4790069882161755</v>
       </c>
       <c r="DS1" t="n">
-        <v>0.04882568489419184</v>
+        <v>0.02071737888482309</v>
       </c>
       <c r="DT1" t="n">
-        <v>0.02177475009122067</v>
+        <v>0.006998693645683568</v>
       </c>
       <c r="DU1" t="n">
-        <v>0.03451821951901787</v>
+        <v>0.1429026578352088</v>
       </c>
       <c r="DV1" t="n">
-        <v>0.03765331088426607</v>
+        <v>0.2055579756700784</v>
       </c>
       <c r="DW1" t="n">
-        <v>0.04262683286272918</v>
+        <v>0.2212217746838939</v>
       </c>
       <c r="DX1" t="n">
-        <v>0.04767323033671755</v>
+        <v>0.2323092003043224</v>
       </c>
       <c r="DY1" t="n">
-        <v>0.05283484566834083</v>
+        <v>0.2499314821110706</v>
       </c>
       <c r="DZ1" t="n">
-        <v>0.05782130077737613</v>
+        <v>0.2750479784935967</v>
       </c>
       <c r="EA1" t="n">
-        <v>0.06252351830631808</v>
+        <v>0.3094975837299574</v>
       </c>
       <c r="EB1" t="n">
-        <v>0.06662732381297808</v>
+        <v>0.3537432441295545</v>
       </c>
       <c r="EC1" t="n">
-        <v>0.06675581318038414</v>
+        <v>0.407467986946694</v>
       </c>
       <c r="ED1" t="n">
-        <v>0.211369021990414</v>
+        <v>0.4643534388184249</v>
       </c>
       <c r="EE1" t="n">
-        <v>2.348338186791202</v>
+        <v>0.5175168591125281</v>
       </c>
       <c r="EF1" t="n">
-        <v>6.694412841132394</v>
+        <v>0.5607929796354572</v>
       </c>
       <c r="EG1" t="n">
-        <v>3.82154269114285</v>
+        <v>0.5887294130546302</v>
       </c>
       <c r="EH1" t="n">
-        <v>-2.82674034862071</v>
+        <v>0.5965866504444072</v>
       </c>
       <c r="EI1" t="n">
-        <v>0.02560632153172512</v>
+        <v>0.5800633426436599</v>
       </c>
       <c r="EJ1" t="n">
-        <v>1.163065809265233</v>
+        <v>0.5406655024269714</v>
       </c>
       <c r="EK1" t="n">
-        <v>-0.7457519449646375</v>
+        <v>0.487417710369573</v>
       </c>
       <c r="EL1" t="n">
-        <v>0.223652961555777</v>
+        <v>0.4282378856154016</v>
       </c>
       <c r="EM1" t="n">
-        <v>0.08686974886531118</v>
+        <v>0.3694949909227493</v>
       </c>
       <c r="EN1" t="n">
-        <v>-0.05377449801541131</v>
+        <v>0.3160090326642657</v>
       </c>
       <c r="EO1" t="n">
-        <v>0.05061803818264074</v>
+        <v>0.2710510608269572</v>
       </c>
       <c r="EP1" t="n">
-        <v>0.009272493083362563</v>
+        <v>0.236343169012188</v>
       </c>
       <c r="EQ1" t="n">
-        <v>0.01541782799955795</v>
+        <v>0.2120728826732369</v>
       </c>
       <c r="ER1" t="n">
-        <v>0.0157489105472473</v>
+        <v>0.1965729454170352</v>
       </c>
       <c r="ES1" t="n">
-        <v>0.01933817694688515</v>
+        <v>0.1875020672716899</v>
       </c>
       <c r="ET1" t="n">
-        <v>0.02512562839607424</v>
+        <v>0.1828742340010866</v>
       </c>
       <c r="EU1" t="n">
-        <v>0.03257801327591208</v>
+        <v>0.1810957624544336</v>
       </c>
       <c r="EV1" t="n">
-        <v>0.04112881550720682</v>
+        <v>0.1809678681520107</v>
       </c>
       <c r="EW1" t="n">
-        <v>0.05034061713167021</v>
+        <v>0.1816866652851696</v>
       </c>
       <c r="EX1" t="n">
-        <v>0.05931141114150257</v>
+        <v>0.1828439873765396</v>
       </c>
       <c r="EY1" t="n">
-        <v>0.06712857477572612</v>
+        <v>0.1842659915867145</v>
       </c>
       <c r="EZ1" t="n">
-        <v>0.1266566551540786</v>
+        <v>0.1856770473987406</v>
       </c>
       <c r="FA1" t="n">
-        <v>1.641665372352978</v>
+        <v>0.1869305961902175</v>
       </c>
       <c r="FB1" t="n">
-        <v>6.070940695961876</v>
+        <v>0.1880549677413868</v>
       </c>
       <c r="FC1" t="n">
-        <v>5.19394232633665</v>
+        <v>0.1892533802351316</v>
       </c>
       <c r="FD1" t="n">
-        <v>-2.190116598211169</v>
+        <v>0.1909039402569758</v>
       </c>
       <c r="FE1" t="n">
-        <v>-0.9068040418132981</v>
+        <v>0.1935606130457446</v>
       </c>
       <c r="FF1" t="n">
-        <v>1.535246547036871</v>
+        <v>0.1995071640634205</v>
       </c>
       <c r="FG1" t="n">
-        <v>-0.6254761766738116</v>
+        <v>0.2128298814766383</v>
       </c>
       <c r="FH1" t="n">
-        <v>0.07291091417540338</v>
+        <v>0.2375965212290991</v>
       </c>
       <c r="FI1" t="n">
-        <v>0.2315845224758989</v>
+        <v>0.2778428597308977</v>
       </c>
       <c r="FJ1" t="n">
-        <v>-0.0456056376160079</v>
+        <v>0.3315925739449356</v>
       </c>
       <c r="FK1" t="n">
-        <v>0.08602638922231602</v>
+        <v>0.3852799617816727</v>
       </c>
       <c r="FL1" t="n">
-        <v>0.04520452243953552</v>
+        <v>0.4238177271458321</v>
       </c>
       <c r="FM1" t="n">
-        <v>0.04354435253025005</v>
+        <v>0.4316320764392712</v>
       </c>
       <c r="FN1" t="n">
-        <v>0.04132621755980136</v>
+        <v>0.4018687969749364</v>
       </c>
       <c r="FO1" t="n">
-        <v>0.0389108258020147</v>
+        <v>0.3491745015933415</v>
       </c>
       <c r="FP1" t="n">
-        <v>0.0378988495447191</v>
+        <v>0.2896400374797183</v>
       </c>
       <c r="FQ1" t="n">
-        <v>0.0376329863491967</v>
+        <v>0.2374432731194235</v>
       </c>
       <c r="FR1" t="n">
-        <v>0.03801710978197621</v>
+        <v>0.2012432424138124</v>
       </c>
       <c r="FS1" t="n">
-        <v>0.03894818654167803</v>
+        <v>0.1806349092914229</v>
       </c>
       <c r="FT1" t="n">
-        <v>0.03997273071447922</v>
+        <v>0.1582037325166215</v>
       </c>
       <c r="FU1" t="n">
-        <v>0.04220312297866679</v>
+        <v>0.09289713384861936</v>
       </c>
       <c r="FV1" t="n">
-        <v>0.05504986803119841</v>
+        <v>0.02483220725811455</v>
       </c>
       <c r="FW1" t="n">
-        <v>1.05763052184469</v>
+        <v>0.1895340725313307</v>
       </c>
       <c r="FX1" t="n">
-        <v>5.199544025677681</v>
+        <v>0.7469334201545866</v>
       </c>
       <c r="FY1" t="n">
-        <v>6.205543357081423</v>
+        <v>1.155948003876334</v>
       </c>
       <c r="FZ1" t="n">
-        <v>-1.107276770096579</v>
+        <v>0.7365847953533297</v>
       </c>
       <c r="GA1" t="n">
-        <v>-1.847057985764238</v>
+        <v>0.1045428151892934</v>
       </c>
       <c r="GB1" t="n">
-        <v>1.641030220863206</v>
+        <v>-0.1204143221867314</v>
       </c>
       <c r="GC1" t="n">
-        <v>-0.3518980021502474</v>
+        <v>-0.02085875850828773</v>
       </c>
       <c r="GD1" t="n">
-        <v>-0.1753806005020255</v>
+        <v>0.09179052204975477</v>
       </c>
       <c r="GE1" t="n">
-        <v>0.3178290131689149</v>
+        <v>0.1273743302489425</v>
       </c>
       <c r="GF1" t="n">
-        <v>-0.06448130468333391</v>
+        <v>0.1387595873266617</v>
       </c>
       <c r="GG1" t="n">
-        <v>0.06717822795715045</v>
+        <v>0.151275114154851</v>
       </c>
       <c r="GH1" t="n">
-        <v>0.04353006753603979</v>
+        <v>0.1702810911146374</v>
       </c>
       <c r="GI1" t="n">
-        <v>0.03293513282372772</v>
+        <v>0.1972814792593038</v>
       </c>
       <c r="GJ1" t="n">
-        <v>0.03166293214847855</v>
+        <v>0.2336658082160792</v>
       </c>
       <c r="GK1" t="n">
-        <v>0.02580736574857726</v>
+        <v>0.2791674423820314</v>
       </c>
       <c r="GL1" t="n">
-        <v>0.02088867782995732</v>
+        <v>0.3319887237356144</v>
       </c>
       <c r="GM1" t="n">
-        <v>0.01597930428327508</v>
+        <v>0.3885855462535974</v>
       </c>
       <c r="GN1" t="n">
-        <v>0.01146124331564931</v>
+        <v>0.4416138539839201</v>
       </c>
       <c r="GO1" t="n">
-        <v>0.007560044156005212</v>
+        <v>0.4842577113531088</v>
       </c>
       <c r="GP1" t="n">
-        <v>0.004495512400127485</v>
+        <v>0.5109575121425449</v>
       </c>
       <c r="GQ1" t="n">
-        <v>0.002492407963564571</v>
+        <v>0.5174099794884673</v>
       </c>
       <c r="GR1" t="n">
-        <v>0.001774904954790893</v>
+        <v>0.5002555446268669</v>
+      </c>
+      <c r="GS1" t="n">
+        <v>0.4621394361032337</v>
+      </c>
+      <c r="GT1" t="n">
+        <v>0.4104541151877527</v>
+      </c>
+      <c r="GU1" t="n">
+        <v>0.3518392954970857</v>
+      </c>
+      <c r="GV1" t="n">
+        <v>0.2920948272399349</v>
+      </c>
+      <c r="GW1" t="n">
+        <v>0.2361806972170417</v>
+      </c>
+      <c r="GX1" t="n">
+        <v>0.1882170288211872</v>
+      </c>
+      <c r="GY1" t="n">
+        <v>0.151249970702058</v>
+      </c>
+      <c r="GZ1" t="n">
+        <v>0.1249455659186249</v>
+      </c>
+      <c r="HA1" t="n">
+        <v>0.1072225576244501</v>
+      </c>
+      <c r="HB1" t="n">
+        <v>0.09616935515549127</v>
+      </c>
+      <c r="HC1" t="n">
+        <v>0.09007133338348071</v>
+      </c>
+      <c r="HD1" t="n">
+        <v>0.08741083271592691</v>
+      </c>
+      <c r="HE1" t="n">
+        <v>0.08686715909611446</v>
+      </c>
+      <c r="HF1" t="n">
+        <v>0.08735101716187044</v>
+      </c>
+      <c r="HG1" t="n">
+        <v>0.08837995759011077</v>
+      </c>
+      <c r="HH1" t="n">
+        <v>0.08969674459306777</v>
+      </c>
+      <c r="HI1" t="n">
+        <v>0.09110195480305976</v>
+      </c>
+      <c r="HJ1" t="n">
+        <v>0.09248441833857236</v>
+      </c>
+      <c r="HK1" t="n">
+        <v>0.09382121880425831</v>
+      </c>
+      <c r="HL1" t="n">
+        <v>0.09517769329093712</v>
+      </c>
+      <c r="HM1" t="n">
+        <v>0.09670743237559577</v>
+      </c>
+      <c r="HN1" t="n">
+        <v>0.09801300671616976</v>
+      </c>
+      <c r="HO1" t="n">
+        <v>0.1007093809256436</v>
+      </c>
+      <c r="HP1" t="n">
+        <v>0.1092364300252007</v>
+      </c>
+      <c r="HQ1" t="n">
+        <v>0.1270700880248033</v>
+      </c>
+      <c r="HR1" t="n">
+        <v>0.1566457733806956</v>
+      </c>
+      <c r="HS1" t="n">
+        <v>0.1993583889954054</v>
+      </c>
+      <c r="HT1" t="n">
+        <v>0.2545503149736685</v>
+      </c>
+      <c r="HU1" t="n">
+        <v>0.3094159055105825</v>
+      </c>
+      <c r="HV1" t="n">
+        <v>0.3465814842450384</v>
+      </c>
+      <c r="HW1" t="n">
+        <v>0.3529910865604817</v>
+      </c>
+      <c r="HX1" t="n">
+        <v>0.3241907880704857</v>
+      </c>
+      <c r="HY1" t="n">
+        <v>0.2720385696210623</v>
+      </c>
+      <c r="HZ1" t="n">
+        <v>0.2122452413334299</v>
+      </c>
+      <c r="IA1" t="n">
+        <v>0.1602098518443742</v>
+      </c>
+      <c r="IB1" t="n">
+        <v>0.1244049859072839</v>
+      </c>
+      <c r="IC1" t="n">
+        <v>0.1042201788659034</v>
+      </c>
+      <c r="ID1" t="n">
+        <v>0.08434130352170324</v>
+      </c>
+      <c r="IE1" t="n">
+        <v>-0.006099862572274744</v>
+      </c>
+      <c r="IF1" t="n">
+        <v>-0.06338669662462808</v>
+      </c>
+      <c r="IG1" t="n">
+        <v>0.08142212629479541</v>
+      </c>
+      <c r="IH1" t="n">
+        <v>0.5163871115772914</v>
+      </c>
+      <c r="II1" t="n">
+        <v>1.077548306131266</v>
+      </c>
+      <c r="IJ1" t="n">
+        <v>0.9236513036077044</v>
+      </c>
+      <c r="IK1" t="n">
+        <v>0.2566829135897345</v>
+      </c>
+      <c r="IL1" t="n">
+        <v>-0.1193340608088316</v>
+      </c>
+      <c r="IM1" t="n">
+        <v>-0.08541193174789187</v>
+      </c>
+      <c r="IN1" t="n">
+        <v>0.04182913337583086</v>
+      </c>
+      <c r="IO1" t="n">
+        <v>0.09834419835166541</v>
+      </c>
+      <c r="IP1" t="n">
+        <v>0.1134131389444009</v>
+      </c>
+      <c r="IQ1" t="n">
+        <v>0.1229959040552238</v>
+      </c>
+      <c r="IR1" t="n">
+        <v>0.1410564449621331</v>
+      </c>
+      <c r="IS1" t="n">
+        <v>0.1664865430061712</v>
+      </c>
+      <c r="IT1" t="n">
+        <v>0.2010267820939936</v>
+      </c>
+      <c r="IU1" t="n">
+        <v>0.2452222904777935</v>
+      </c>
+      <c r="IV1" t="n">
+        <v>0.2975406906655201</v>
+      </c>
+      <c r="IW1" t="n">
+        <v>0.3547537852999642</v>
+      </c>
+      <c r="IX1" t="n">
+        <v>0.4112780278450247</v>
+      </c>
+      <c r="IY1" t="n">
+        <v>0.4591736571113053</v>
+      </c>
+      <c r="IZ1" t="n">
+        <v>0.4920730298729379</v>
+      </c>
+      <c r="JA1" t="n">
+        <v>0.5054284318823045</v>
+      </c>
+      <c r="JB1" t="n">
+        <v>0.4963441960815999</v>
+      </c>
+      <c r="JC1" t="n">
+        <v>0.4639464512951625</v>
+      </c>
+      <c r="JD1" t="n">
+        <v>0.4155446210871493</v>
+      </c>
+      <c r="JE1" t="n">
+        <v>0.3589221708191981</v>
+      </c>
+      <c r="JF1" t="n">
+        <v>0.3005312047614457</v>
+      </c>
+      <c r="JG1" t="n">
+        <v>0.2455001032326451</v>
+      </c>
+      <c r="JH1" t="n">
+        <v>0.1976283318540078</v>
+      </c>
+      <c r="JI1" t="n">
+        <v>0.1593827040028756</v>
+      </c>
+      <c r="JJ1" t="n">
+        <v>0.1318263459840857</v>
+      </c>
+      <c r="JK1" t="n">
+        <v>0.1136927627500454</v>
+      </c>
+      <c r="JL1" t="n">
+        <v>0.1026816511730897</v>
+      </c>
+      <c r="JM1" t="n">
+        <v>0.09680913188141697</v>
+      </c>
+      <c r="JN1" t="n">
+        <v>0.09443544173303588</v>
+      </c>
+      <c r="JO1" t="n">
+        <v>0.09426493381576467</v>
+      </c>
+      <c r="JP1" t="n">
+        <v>0.09534607744723093</v>
+      </c>
+      <c r="JQ1" t="n">
+        <v>0.09707145817487162</v>
+      </c>
+      <c r="JR1" t="n">
+        <v>0.09921308470109981</v>
+      </c>
+      <c r="JS1" t="n">
+        <v>0.1016331237981905</v>
+      </c>
+      <c r="JT1" t="n">
+        <v>0.1040128921041367</v>
+      </c>
+      <c r="JU1" t="n">
+        <v>0.1062365731575204</v>
+      </c>
+      <c r="JV1" t="n">
+        <v>0.1084047093065248</v>
+      </c>
+      <c r="JW1" t="n">
+        <v>0.110840254074553</v>
+      </c>
+      <c r="JX1" t="n">
+        <v>0.1140897244540639</v>
+      </c>
+      <c r="JY1" t="n">
+        <v>0.1188705364987792</v>
+      </c>
+      <c r="JZ1" t="n">
+        <v>0.1269134457754051</v>
+      </c>
+      <c r="KA1" t="n">
+        <v>0.1434487904935818</v>
+      </c>
+      <c r="KB1" t="n">
+        <v>0.172440219046663</v>
+      </c>
+      <c r="KC1" t="n">
+        <v>0.2156687201846407</v>
+      </c>
+      <c r="KD1" t="n">
+        <v>0.2726777931464971</v>
+      </c>
+      <c r="KE1" t="n">
+        <v>0.3305490738761969</v>
+      </c>
+      <c r="KF1" t="n">
+        <v>0.3704191743292911</v>
+      </c>
+      <c r="KG1" t="n">
+        <v>0.3805904744548503</v>
+      </c>
+      <c r="KH1" t="n">
+        <v>0.3568150879576155</v>
+      </c>
+      <c r="KI1" t="n">
+        <v>0.3060375571972589</v>
+      </c>
+      <c r="KJ1" t="n">
+        <v>0.247918512143178</v>
+      </c>
+      <c r="KK1" t="n">
+        <v>0.197418614933071</v>
+      </c>
+      <c r="KL1" t="n">
+        <v>0.1619508572797769</v>
+      </c>
+      <c r="KM1" t="n">
+        <v>0.141901339270495</v>
+      </c>
+      <c r="KN1" t="n">
+        <v>0.1226216025123674</v>
+      </c>
+      <c r="KO1" t="n">
+        <v>0.07338663858699568</v>
+      </c>
+      <c r="KP1" t="n">
+        <v>-0.0106898990874677</v>
+      </c>
+      <c r="KQ1" t="n">
+        <v>0.06336213226825468</v>
+      </c>
+      <c r="KR1" t="n">
+        <v>0.5170084451033725</v>
+      </c>
+      <c r="KS1" t="n">
+        <v>1.089328225439675</v>
+      </c>
+      <c r="KT1" t="n">
+        <v>0.947923548931489</v>
+      </c>
+      <c r="KU1" t="n">
+        <v>0.2831791246060915</v>
+      </c>
+      <c r="KV1" t="n">
+        <v>-0.05593425723495338</v>
+      </c>
+      <c r="KW1" t="n">
+        <v>-0.003190086285730928</v>
+      </c>
+      <c r="KX1" t="n">
+        <v>0.1238259568250713</v>
+      </c>
+      <c r="KY1" t="n">
+        <v>0.1679677590553773</v>
+      </c>
+      <c r="KZ1" t="n">
+        <v>0.1812554166364299</v>
+      </c>
+      <c r="LA1" t="n">
+        <v>0.1956501157361982</v>
+      </c>
+      <c r="LB1" t="n">
+        <v>0.216561072784517</v>
+      </c>
+      <c r="LC1" t="n">
+        <v>0.2462634051693135</v>
+      </c>
+      <c r="LD1" t="n">
+        <v>0.2860415873564418</v>
+      </c>
+      <c r="LE1" t="n">
+        <v>0.3350533554518275</v>
+      </c>
+      <c r="LF1" t="n">
+        <v>0.3906282674690423</v>
+      </c>
+      <c r="LG1" t="n">
+        <v>0.4483758940045166</v>
+      </c>
+      <c r="LH1" t="n">
+        <v>0.5021858182375392</v>
+      </c>
+      <c r="LI1" t="n">
+        <v>0.5442276359302568</v>
+      </c>
+      <c r="LJ1" t="n">
+        <v>0.5664420476782466</v>
+      </c>
+      <c r="LK1" t="n">
+        <v>0.5658816435115502</v>
+      </c>
+      <c r="LL1" t="n">
+        <v>0.5428265656880633</v>
+      </c>
+      <c r="LM1" t="n">
+        <v>0.5005184207458646</v>
+      </c>
+      <c r="LN1" t="n">
+        <v>0.445184404864395</v>
+      </c>
+      <c r="LO1" t="n">
+        <v>0.3856316217157028</v>
+      </c>
+      <c r="LP1" t="n">
+        <v>0.3289286902973728</v>
+      </c>
+      <c r="LQ1" t="n">
+        <v>0.2799422295389499</v>
+      </c>
+      <c r="LR1" t="n">
+        <v>0.2414780311216626</v>
+      </c>
+      <c r="LS1" t="n">
+        <v>0.2141186712506641</v>
+      </c>
+      <c r="LT1" t="n">
+        <v>0.1962871387771067</v>
+      </c>
+      <c r="LU1" t="n">
+        <v>0.1858300428763361</v>
+      </c>
+      <c r="LV1" t="n">
+        <v>0.1806456369540403</v>
+      </c>
+      <c r="LW1" t="n">
+        <v>0.178884811727893</v>
+      </c>
+      <c r="LX1" t="n">
+        <v>0.1791558433747264</v>
+      </c>
+      <c r="LY1" t="n">
+        <v>0.1805243935305322</v>
+      </c>
+      <c r="LZ1" t="n">
+        <v>0.1825190644886234</v>
+      </c>
+      <c r="MA1" t="n">
+        <v>0.1848626771241608</v>
+      </c>
+      <c r="MB1" t="n">
+        <v>0.1872434108567654</v>
+      </c>
+      <c r="MC1" t="n">
+        <v>0.189513156086551</v>
+      </c>
+      <c r="MD1" t="n">
+        <v>0.1916997945951543</v>
+      </c>
+      <c r="ME1" t="n">
+        <v>0.1940073659126872</v>
+      </c>
+      <c r="MF1" t="n">
+        <v>0.1968160673177359</v>
+      </c>
+      <c r="MG1" t="n">
+        <v>0.2006486895116383</v>
+      </c>
+      <c r="MH1" t="n">
+        <v>0.2065752953853852</v>
+      </c>
+      <c r="MI1" t="n">
+        <v>0.2195276714927637</v>
+      </c>
+      <c r="MJ1" t="n">
+        <v>0.2439641413426278</v>
+      </c>
+      <c r="MK1" t="n">
+        <v>0.2826052999644605</v>
+      </c>
+      <c r="ML1" t="n">
+        <v>0.3366939874288045</v>
+      </c>
+      <c r="MM1" t="n">
+        <v>0.3965713046961774</v>
+      </c>
+      <c r="MN1" t="n">
+        <v>0.4407752517814332</v>
+      </c>
+      <c r="MO1" t="n">
+        <v>0.4554508151040634</v>
+      </c>
+      <c r="MP1" t="n">
+        <v>0.4356160223050392</v>
+      </c>
+      <c r="MQ1" t="n">
+        <v>0.386706336199967</v>
+      </c>
+      <c r="MR1" t="n">
+        <v>0.328585341764705</v>
+      </c>
+      <c r="MS1" t="n">
+        <v>0.278397014514521</v>
+      </c>
+      <c r="MT1" t="n">
+        <v>0.244178148482387</v>
+      </c>
+      <c r="MU1" t="n">
+        <v>0.224938636459028</v>
+      </c>
+      <c r="MV1" t="n">
+        <v>0.2055050643866513</v>
+      </c>
+      <c r="MW1" t="n">
+        <v>0.1463404712018454</v>
+      </c>
+      <c r="MX1" t="n">
+        <v>0.07577267825802812</v>
+      </c>
+      <c r="MY1" t="n">
+        <v>0.2272399046582894</v>
+      </c>
+      <c r="MZ1" t="n">
+        <v>0.7816273074874358</v>
+      </c>
+      <c r="NA1" t="n">
+        <v>1.200061897109337</v>
+      </c>
+      <c r="NB1" t="n">
+        <v>0.7782108949889162</v>
+      </c>
+      <c r="NC1" t="n">
+        <v>0.1701375446509872</v>
+      </c>
+      <c r="ND1" t="n">
+        <v>0.01041437274471349</v>
+      </c>
+      <c r="NE1" t="n">
+        <v>0.1342545248932889</v>
+      </c>
+      <c r="NF1" t="n">
+        <v>0.2231140615511742</v>
+      </c>
+      <c r="NG1" t="n">
+        <v>0.2465277790378079</v>
+      </c>
+      <c r="NH1" t="n">
+        <v>0.2560564309697921</v>
+      </c>
+      <c r="NI1" t="n">
+        <v>0.272746398593995</v>
+      </c>
+      <c r="NJ1" t="n">
+        <v>0.2967212128301885</v>
+      </c>
+      <c r="NK1" t="n">
+        <v>0.3302616400872426</v>
+      </c>
+      <c r="NL1" t="n">
+        <v>0.3738523266131122</v>
+      </c>
+      <c r="NM1" t="n">
+        <v>0.4270100655021695</v>
+      </c>
+      <c r="NN1" t="n">
+        <v>0.4848191812629785</v>
+      </c>
+      <c r="NO1" t="n">
+        <v>0.5392477982168522</v>
+      </c>
+      <c r="NP1" t="n">
+        <v>0.5832854778231521</v>
+      </c>
+      <c r="NQ1" t="n">
+        <v>0.6109705194473652</v>
+      </c>
+      <c r="NR1" t="n">
+        <v>0.6173899603610988</v>
+      </c>
+      <c r="NS1" t="n">
+        <v>0.5982476427546883</v>
+      </c>
+      <c r="NT1" t="n">
+        <v>0.5567668505768623</v>
+      </c>
+      <c r="NU1" t="n">
+        <v>0.5026869403925247</v>
+      </c>
+      <c r="NV1" t="n">
+        <v>0.4441604911074852</v>
+      </c>
+      <c r="NW1" t="n">
+        <v>0.3875837297531128</v>
+      </c>
+      <c r="NX1" t="n">
+        <v>0.3375965314863381</v>
+      </c>
+      <c r="NY1" t="n">
+        <v>0.2970824195896505</v>
+      </c>
+      <c r="NZ1" t="n">
+        <v>0.2671685766636796</v>
+      </c>
+      <c r="OA1" t="n">
+        <v>0.2473398656508259</v>
+      </c>
+      <c r="OB1" t="n">
+        <v>0.2354028155105347</v>
+      </c>
+      <c r="OC1" t="n">
+        <v>0.2289919316792906</v>
+      </c>
+      <c r="OD1" t="n">
+        <v>0.2261839051043498</v>
+      </c>
+      <c r="OE1" t="n">
+        <v>0.2254976122437402</v>
+      </c>
+      <c r="OF1" t="n">
+        <v>0.2258941150662609</v>
+      </c>
+      <c r="OG1" t="n">
+        <v>0.2267766610514827</v>
+      </c>
+      <c r="OH1" t="n">
+        <v>0.2279223113953902</v>
+      </c>
+      <c r="OI1" t="n">
+        <v>0.2291106788703169</v>
+      </c>
+      <c r="OJ1" t="n">
+        <v>0.2301969864748747</v>
+      </c>
+      <c r="OK1" t="n">
+        <v>0.2311944306091903</v>
+      </c>
+      <c r="OL1" t="n">
+        <v>0.2322740806922156</v>
+      </c>
+      <c r="OM1" t="n">
+        <v>0.233764879161729</v>
+      </c>
+      <c r="ON1" t="n">
+        <v>0.2361354306081602</v>
+      </c>
+      <c r="OO1" t="n">
+        <v>0.2418578792423468</v>
+      </c>
+      <c r="OP1" t="n">
+        <v>0.255007484051778</v>
+      </c>
+      <c r="OQ1" t="n">
+        <v>0.2797877451463775</v>
+      </c>
+      <c r="OR1" t="n">
+        <v>0.320697263114149</v>
+      </c>
+      <c r="OS1" t="n">
+        <v>0.3763644935351048</v>
+      </c>
+      <c r="OT1" t="n">
+        <v>0.4305128205559365</v>
+      </c>
+      <c r="OU1" t="n">
+        <v>0.4671297044541472</v>
+      </c>
+      <c r="OV1" t="n">
+        <v>0.4725031590314541</v>
+      </c>
+      <c r="OW1" t="n">
+        <v>0.4388767003722631</v>
+      </c>
+      <c r="OX1" t="n">
+        <v>0.3835143642906821</v>
+      </c>
+      <c r="OY1" t="n">
+        <v>0.3269827258526073</v>
+      </c>
+      <c r="OZ1" t="n">
+        <v>0.2819177272434495</v>
+      </c>
+      <c r="PA1" t="n">
+        <v>0.2530145975921137</v>
+      </c>
+      <c r="PB1" t="n">
+        <v>0.2439636271181312</v>
+      </c>
+      <c r="PC1" t="n">
+        <v>0.2024925114194693</v>
+      </c>
+      <c r="PD1" t="n">
+        <v>0.1148187241758208</v>
+      </c>
+      <c r="PE1" t="n">
+        <v>0.1100429876393554</v>
+      </c>
+      <c r="PF1" t="n">
+        <v>0.4747023907096501</v>
+      </c>
+      <c r="PG1" t="n">
+        <v>1.077925523407568</v>
+      </c>
+      <c r="PH1" t="n">
+        <v>1.052412561919476</v>
+      </c>
+      <c r="PI1" t="n">
+        <v>0.3961307930336455</v>
+      </c>
+      <c r="PJ1" t="n">
+        <v>-0.004052174863745324</v>
+      </c>
+      <c r="PK1" t="n">
+        <v>0.02560415205346814</v>
+      </c>
+      <c r="PL1" t="n">
+        <v>0.153439630430519</v>
+      </c>
+      <c r="PM1" t="n">
+        <v>0.2020928677672677</v>
+      </c>
+      <c r="PN1" t="n">
+        <v>0.2131132988461585</v>
+      </c>
+      <c r="PO1" t="n">
+        <v>0.2228854960358932</v>
+      </c>
+      <c r="PP1" t="n">
+        <v>0.2406821610719417</v>
+      </c>
+      <c r="PQ1" t="n">
+        <v>0.2662799183807132</v>
+      </c>
+      <c r="PR1" t="n">
+        <v>0.3017010856088401</v>
+      </c>
+      <c r="PS1" t="n">
+        <v>0.3467258617977728</v>
+      </c>
+      <c r="PT1" t="n">
+        <v>0.3997701147184572</v>
+      </c>
+      <c r="PU1" t="n">
+        <v>0.4552031966591968</v>
+      </c>
+      <c r="PV1" t="n">
+        <v>0.5055487035931282</v>
+      </c>
+      <c r="PW1" t="n">
+        <v>0.5440906082672049</v>
+      </c>
+      <c r="PX1" t="n">
+        <v>0.5648771371047983</v>
+      </c>
+      <c r="PY1" t="n">
+        <v>0.5623512160764423</v>
+      </c>
+      <c r="PZ1" t="n">
+        <v>0.5347462339958667</v>
+      </c>
+      <c r="QA1" t="n">
+        <v>0.4895989673326465</v>
+      </c>
+      <c r="QB1" t="n">
+        <v>0.4343973566809738</v>
+      </c>
+      <c r="QC1" t="n">
+        <v>0.3756420826294782</v>
+      </c>
+      <c r="QD1" t="n">
+        <v>0.318846811878427</v>
+      </c>
+      <c r="QE1" t="n">
+        <v>0.2685381972397262</v>
+      </c>
+      <c r="QF1" t="n">
+        <v>0.2282558776369197</v>
+      </c>
+      <c r="QG1" t="n">
+        <v>0.1997386204495826</v>
+      </c>
+      <c r="QH1" t="n">
+        <v>0.1809946455903702</v>
+      </c>
+      <c r="QI1" t="n">
+        <v>0.1695250416283546</v>
+      </c>
+      <c r="QJ1" t="n">
+        <v>0.1631961076268979</v>
+      </c>
+      <c r="QK1" t="n">
+        <v>0.1602391076679442</v>
+      </c>
+      <c r="QL1" t="n">
+        <v>0.1592502708520179</v>
+      </c>
+      <c r="QM1" t="n">
+        <v>0.1591907912982243</v>
+      </c>
+      <c r="QN1" t="n">
+        <v>0.1593868283797935</v>
+      </c>
+      <c r="QO1" t="n">
+        <v>0.1595396044617018</v>
+      </c>
+      <c r="QP1" t="n">
+        <v>0.1598132881256582</v>
+      </c>
+      <c r="QQ1" t="n">
+        <v>0.1604912594578919</v>
+      </c>
+      <c r="QR1" t="n">
+        <v>0.1607328623730432</v>
+      </c>
+      <c r="QS1" t="n">
+        <v>0.1602865649870175</v>
+      </c>
+      <c r="QT1" t="n">
+        <v>0.1597492865214282</v>
+      </c>
+      <c r="QU1" t="n">
+        <v>0.160566397303597</v>
+      </c>
+      <c r="QV1" t="n">
+        <v>0.1650317187665538</v>
+      </c>
+      <c r="QW1" t="n">
+        <v>0.1762875234490361</v>
+      </c>
+      <c r="QX1" t="n">
+        <v>0.1983245349954898</v>
+      </c>
+      <c r="QY1" t="n">
+        <v>0.2358612856374518</v>
+      </c>
+      <c r="QZ1" t="n">
+        <v>0.2879117545328129</v>
+      </c>
+      <c r="RA1" t="n">
+        <v>0.3428718219603091</v>
+      </c>
+      <c r="RB1" t="n">
+        <v>0.3848883329394128</v>
+      </c>
+      <c r="RC1" t="n">
+        <v>0.3955151307140429</v>
+      </c>
+      <c r="RD1" t="n">
+        <v>0.3701406353476573</v>
+      </c>
+      <c r="RE1" t="n">
+        <v>0.3194364035431504</v>
+      </c>
+      <c r="RF1" t="n">
+        <v>0.2596494473544122</v>
+      </c>
+      <c r="RG1" t="n">
+        <v>0.2086238780649806</v>
+      </c>
+      <c r="RH1" t="n">
+        <v>0.1753852307549775</v>
+      </c>
+      <c r="RI1" t="n">
+        <v>0.1574282534479334</v>
+      </c>
+      <c r="RJ1" t="n">
+        <v>0.1342146797379792</v>
+      </c>
+      <c r="RK1" t="n">
+        <v>0.06728798117464647</v>
+      </c>
+      <c r="RL1" t="n">
+        <v>0.006395674415578847</v>
+      </c>
+      <c r="RM1" t="n">
+        <v>0.2108765325583272</v>
+      </c>
+      <c r="RN1" t="n">
+        <v>0.799669501379946</v>
+      </c>
+      <c r="RO1" t="n">
+        <v>1.114856863366805</v>
+      </c>
+      <c r="RP1" t="n">
+        <v>0.5989511004862169</v>
+      </c>
+      <c r="RQ1" t="n">
+        <v>0.02344056783370206</v>
+      </c>
+      <c r="RR1" t="n">
+        <v>-0.1017506689996707</v>
+      </c>
+      <c r="RS1" t="n">
+        <v>0.02636768239571221</v>
+      </c>
+      <c r="RT1" t="n">
+        <v>0.1110900464960492</v>
+      </c>
+      <c r="RU1" t="n">
+        <v>0.1321266400606966</v>
+      </c>
+      <c r="RV1" t="n">
+        <v>0.1401672544993053</v>
+      </c>
+      <c r="RW1" t="n">
+        <v>0.1544447201054562</v>
+      </c>
+      <c r="RX1" t="n">
+        <v>0.1756177291869969</v>
+      </c>
+      <c r="RY1" t="n">
+        <v>0.2060417333509809</v>
+      </c>
+      <c r="RZ1" t="n">
+        <v>0.2463121799656381</v>
+      </c>
+      <c r="SA1" t="n">
+        <v>0.2957299930612081</v>
+      </c>
+      <c r="SB1" t="n">
+        <v>0.3514273726500651</v>
+      </c>
+      <c r="SC1" t="n">
+        <v>0.4058121819300439</v>
+      </c>
+      <c r="SD1" t="n">
+        <v>0.4518168576837477</v>
+      </c>
+      <c r="SE1" t="n">
+        <v>0.4834429925264355</v>
+      </c>
+      <c r="SF1" t="n">
+        <v>0.4957613349060201</v>
       </c>
     </row>
   </sheetData>

</xml_diff>